<commit_message>
correction d'erreurs dans les fichiers de donnees + modif fichier preparation.R
</commit_message>
<xml_diff>
--- a/Donnees/1989 Andalucia Granada.xlsx
+++ b/Donnees/1989 Andalucia Granada.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c2f1b5ee3ad3a97/Desktop/COURS M2 EEET - MP/Méthodes (6ECTS)/Analyse économétrique de la demande/Projet Analyse Econo Demande/Donnees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{3B052623-A9D0-46B3-BAE3-64E79817462D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA3DED8F-898C-4493-8F1E-CF8C9F0E92EA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B76CCD5C-3C3D-490F-863B-DB258A414B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E06F2B33-D09C-4B7C-BBB4-DDA146E24099}"/>
+    <workbookView xWindow="4620" yWindow="1860" windowWidth="16140" windowHeight="11820" xr2:uid="{F39B5C26-F319-4841-B7F3-9DE803F8E0E7}"/>
   </bookViews>
   <sheets>
-    <sheet name="estadisticas (19)" sheetId="1" r:id="rId1"/>
+    <sheet name="estadisticas - 2025-05-04T11175" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Tipo convocatoria</t>
   </si>
@@ -67,64 +67,64 @@
     <t>PART. SOCIALISTA OBRERO ESPAÃ‘OL DE ANDALUCIA</t>
   </si>
   <si>
-    <t>207.503</t>
+    <t>204.596</t>
   </si>
   <si>
     <t>Diputados</t>
   </si>
   <si>
+    <t>PARTIDO POPULAR</t>
+  </si>
+  <si>
+    <t>100.619</t>
+  </si>
+  <si>
     <t>IZQUIERDA UNIDA-CONVOCATORIA POR ANDALUCIA</t>
   </si>
   <si>
-    <t>77.106</t>
-  </si>
-  <si>
-    <t>PARTIDO POPULAR</t>
-  </si>
-  <si>
-    <t>76.561</t>
+    <t>47.067</t>
+  </si>
+  <si>
+    <t>CENTRO DEMOCRATICO Y SOCIAL</t>
+  </si>
+  <si>
+    <t>24.619</t>
   </si>
   <si>
     <t>PARTIDO ANDALUCISTA</t>
   </si>
   <si>
-    <t>24.714</t>
-  </si>
-  <si>
-    <t>CENTRO DEMOCRATICO Y SOCIAL</t>
-  </si>
-  <si>
-    <t>21.110</t>
+    <t>10.824</t>
   </si>
   <si>
     <t>AGRUPACION RUIZ-MATEOS</t>
   </si>
   <si>
-    <t>4.893</t>
+    <t>5.613</t>
   </si>
   <si>
     <t>PARTIDO TRABAJADORES DE ESPAÃ‘A-UNIDAD COMUNISTA</t>
   </si>
   <si>
-    <t>1.504</t>
+    <t>4.310</t>
   </si>
   <si>
     <t>LOS VERDES-LISTA VERDE.</t>
   </si>
   <si>
-    <t>1.343</t>
+    <t>3.833</t>
+  </si>
+  <si>
+    <t>LOS VERDES ECOLOGISTAS</t>
+  </si>
+  <si>
+    <t>2.179</t>
   </si>
   <si>
     <t>PARTIDO SOCIALISTA DE LOS TRABAJADORES</t>
   </si>
   <si>
-    <t>1.271</t>
-  </si>
-  <si>
-    <t>LOS VERDES ECOLOGISTAS.</t>
-  </si>
-  <si>
-    <t>1.153</t>
+    <t>1.042</t>
   </si>
   <si>
     <t>PARTIDO COMUNISTA DEL PUEBLO ANDALUZ</t>
@@ -133,22 +133,13 @@
     <t>FALANGE ESPAÃ‘OLA DE LAS J.O.N.S.</t>
   </si>
   <si>
+    <t>PARTIDO HUMANISTA</t>
+  </si>
+  <si>
     <t>ALIANZA POR LA REPUBLICA</t>
   </si>
   <si>
-    <t>PARTIDO HUMANISTA DE ANDALUCIA</t>
-  </si>
-  <si>
     <t>UNIDAD CENTRISTA-P.E.D.</t>
-  </si>
-  <si>
-    <t>ano</t>
-  </si>
-  <si>
-    <t>etranger</t>
-  </si>
-  <si>
-    <t>oui</t>
   </si>
 </sst>
 </file>
@@ -1008,693 +999,580 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C7E1E4-1712-4829-B257-058CC76F0BE3}">
-  <dimension ref="A1:P16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDF2B00-5462-4C1B-AC25-10A3DD88EB14}">
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>198910</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>50.05</v>
+      </c>
+      <c r="K2">
+        <v>34.4</v>
+      </c>
+      <c r="L2">
+        <v>50.33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="str">
-        <f>LEFT(C2,4)</f>
-        <v>1989</v>
-      </c>
-      <c r="C2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>198910</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2">
-        <v>49.36</v>
-      </c>
-      <c r="L2">
-        <v>36.9</v>
-      </c>
-      <c r="M2">
-        <v>49.54</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>24.61</v>
+      </c>
+      <c r="K3">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="L3">
+        <v>24.75</v>
+      </c>
+      <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c r="O2">
-        <v>5</v>
-      </c>
-      <c r="P2" t="s">
-        <v>42</v>
+      <c r="N3">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B16" si="0">LEFT(C3,4)</f>
-        <v>1989</v>
-      </c>
-      <c r="C3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>198910</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>18</v>
       </c>
-      <c r="K3">
-        <v>18.34</v>
-      </c>
-      <c r="L3">
-        <v>13.71</v>
-      </c>
-      <c r="M3">
-        <v>18.41</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>11.51</v>
+      </c>
+      <c r="K4">
+        <v>7.91</v>
+      </c>
+      <c r="L4">
+        <v>11.58</v>
+      </c>
+      <c r="M4" t="s">
         <v>16</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
-        <v>42</v>
+      <c r="N4">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>198910</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <v>18.21</v>
-      </c>
-      <c r="L4">
-        <v>13.61</v>
-      </c>
-      <c r="M4">
-        <v>18.28</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>6.02</v>
+      </c>
+      <c r="K5">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="L5">
+        <v>6.06</v>
+      </c>
+      <c r="M5" t="s">
         <v>16</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>42</v>
+      <c r="N5">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
         <v>198910</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5">
-        <v>5.88</v>
-      </c>
-      <c r="L5">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="M5">
-        <v>5.9</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6">
+        <v>2.65</v>
+      </c>
+      <c r="K6">
+        <v>1.82</v>
+      </c>
+      <c r="L6">
+        <v>2.66</v>
+      </c>
+      <c r="M6" t="s">
         <v>16</v>
       </c>
-      <c r="O5">
+      <c r="N6">
         <v>0</v>
       </c>
-      <c r="P5" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C6">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <v>198910</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6">
-        <v>5.0199999999999996</v>
-      </c>
-      <c r="L6">
-        <v>3.75</v>
-      </c>
-      <c r="M6">
-        <v>5.04</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7">
+        <v>1.37</v>
+      </c>
+      <c r="K7">
+        <v>0.94</v>
+      </c>
+      <c r="L7">
+        <v>1.38</v>
+      </c>
+      <c r="M7" t="s">
         <v>16</v>
       </c>
-      <c r="O6">
+      <c r="N7">
         <v>0</v>
       </c>
-      <c r="P6" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C7">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>198910</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="L7">
-        <v>0.87</v>
-      </c>
-      <c r="M7">
-        <v>1.17</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8">
+        <v>1.05</v>
+      </c>
+      <c r="K8">
+        <v>0.72</v>
+      </c>
+      <c r="L8">
+        <v>1.06</v>
+      </c>
+      <c r="M8" t="s">
         <v>16</v>
       </c>
-      <c r="O7">
+      <c r="N8">
         <v>0</v>
       </c>
-      <c r="P7" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C8">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
         <v>198910</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>14</v>
-      </c>
-      <c r="I8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8">
-        <v>0.36</v>
-      </c>
-      <c r="L8">
-        <v>0.27</v>
-      </c>
-      <c r="M8">
-        <v>0.36</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <v>0.94</v>
+      </c>
+      <c r="K9">
+        <v>0.64</v>
+      </c>
+      <c r="L9">
+        <v>0.94</v>
+      </c>
+      <c r="M9" t="s">
         <v>16</v>
       </c>
-      <c r="O8">
+      <c r="N9">
         <v>0</v>
       </c>
-      <c r="P8" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C9">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
         <v>198910</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>14</v>
-      </c>
-      <c r="I9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9">
-        <v>0.32</v>
-      </c>
-      <c r="L9">
-        <v>0.24</v>
-      </c>
-      <c r="M9">
-        <v>0.32</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <v>0.53</v>
+      </c>
+      <c r="K10">
+        <v>0.37</v>
+      </c>
+      <c r="L10">
+        <v>0.54</v>
+      </c>
+      <c r="M10" t="s">
         <v>16</v>
       </c>
-      <c r="O9">
+      <c r="N10">
         <v>0</v>
       </c>
-      <c r="P9" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C10">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
         <v>198910</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>14</v>
-      </c>
-      <c r="I10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10">
-        <v>0.3</v>
-      </c>
-      <c r="L10">
-        <v>0.23</v>
-      </c>
-      <c r="M10">
-        <v>0.3</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11">
+        <v>0.25</v>
+      </c>
+      <c r="K11">
+        <v>0.18</v>
+      </c>
+      <c r="L11">
+        <v>0.26</v>
+      </c>
+      <c r="M11" t="s">
         <v>16</v>
       </c>
-      <c r="O10">
+      <c r="N11">
         <v>0</v>
       </c>
-      <c r="P10" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C11">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
         <v>198910</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>14</v>
-      </c>
-      <c r="I11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11">
-        <v>0.27</v>
-      </c>
-      <c r="L11">
-        <v>0.21</v>
-      </c>
-      <c r="M11">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>18</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12">
+        <v>800</v>
+      </c>
+      <c r="J12">
+        <v>0.2</v>
+      </c>
+      <c r="K12">
+        <v>0.13</v>
+      </c>
+      <c r="L12">
+        <v>0.2</v>
+      </c>
+      <c r="M12" t="s">
         <v>16</v>
       </c>
-      <c r="O11">
+      <c r="N12">
         <v>0</v>
       </c>
-      <c r="P11" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C12">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
         <v>198910</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>14</v>
-      </c>
-      <c r="I12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12">
-        <v>705</v>
-      </c>
-      <c r="K12">
-        <v>0.17</v>
-      </c>
-      <c r="L12">
-        <v>0.13</v>
-      </c>
-      <c r="M12">
-        <v>0.17</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13">
+        <v>460</v>
+      </c>
+      <c r="J13">
+        <v>0.11</v>
+      </c>
+      <c r="K13">
+        <v>0.08</v>
+      </c>
+      <c r="L13">
+        <v>0.11</v>
+      </c>
+      <c r="M13" t="s">
         <v>16</v>
       </c>
-      <c r="O12">
+      <c r="N13">
         <v>0</v>
       </c>
-      <c r="P12" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C13">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
         <v>198910</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>14</v>
-      </c>
-      <c r="I13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13">
-        <v>368</v>
-      </c>
-      <c r="K13">
-        <v>0.09</v>
-      </c>
-      <c r="L13">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="M13">
-        <v>0.09</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14">
+        <v>219</v>
+      </c>
+      <c r="J14">
+        <v>0.05</v>
+      </c>
+      <c r="K14">
+        <v>0.04</v>
+      </c>
+      <c r="L14">
+        <v>0.05</v>
+      </c>
+      <c r="M14" t="s">
         <v>16</v>
       </c>
-      <c r="O13">
+      <c r="N14">
         <v>0</v>
       </c>
-      <c r="P13" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
         <v>198910</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>14</v>
-      </c>
-      <c r="I14" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14">
-        <v>216</v>
-      </c>
-      <c r="K14">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15">
+        <v>191</v>
+      </c>
+      <c r="J15">
         <v>0.05</v>
       </c>
-      <c r="L14">
+      <c r="K15">
+        <v>0.03</v>
+      </c>
+      <c r="L15">
+        <v>0.05</v>
+      </c>
+      <c r="M15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>198910</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16">
+        <v>174</v>
+      </c>
+      <c r="J16">
         <v>0.04</v>
       </c>
-      <c r="M14">
-        <v>0.05</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="K16">
+        <v>0.03</v>
+      </c>
+      <c r="L16">
+        <v>0.04</v>
+      </c>
+      <c r="M16" t="s">
         <v>16</v>
       </c>
-      <c r="O14">
+      <c r="N16">
         <v>0</v>
-      </c>
-      <c r="P14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C15">
-        <v>198910</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>14</v>
-      </c>
-      <c r="I15" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15">
-        <v>214</v>
-      </c>
-      <c r="K15">
-        <v>0.05</v>
-      </c>
-      <c r="L15">
-        <v>0.04</v>
-      </c>
-      <c r="M15">
-        <v>0.05</v>
-      </c>
-      <c r="N15" t="s">
-        <v>16</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="C16">
-        <v>198910</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>14</v>
-      </c>
-      <c r="I16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16">
-        <v>160</v>
-      </c>
-      <c r="K16">
-        <v>0.04</v>
-      </c>
-      <c r="L16">
-        <v>0.03</v>
-      </c>
-      <c r="M16">
-        <v>0.04</v>
-      </c>
-      <c r="N16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>